<commit_message>
Agregando Separaciones de gastos
</commit_message>
<xml_diff>
--- a/public/Reservas.xlsx
+++ b/public/Reservas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\booking\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\boocking\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1380CE-3C65-4110-A196-C88C07AAAC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848AB2DC-7526-4243-AFB6-49D15B8F0134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5308,10 +5308,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="N102" sqref="N102"/>
+      <selection pane="bottomLeft" activeCell="M296" sqref="M296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>